<commit_message>
Added new dataseries. 🧩
</commit_message>
<xml_diff>
--- a/data/data_2018-2020.xlsx
+++ b/data/data_2018-2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\research\idaf\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael.beutler/Documents/repos/bbzbl-idaf-data-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E25E92B-C599-457F-AFB7-A3AD74E464DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC514A9-BDD2-054E-8604-5BF9F7213DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{601E68D1-B156-4EC6-9567-408923F44C9F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{601E68D1-B156-4EC6-9567-408923F44C9F}"/>
   </bookViews>
   <sheets>
     <sheet name="2018-2020" sheetId="1" r:id="rId1"/>
@@ -142,10 +142,10 @@
     <t>Teilzeitbeschäftigte Frauen</t>
   </si>
   <si>
-    <t>Geschlechts-spezifisches Verdienstgefälle in Industrie, Baugewerbe und Dienstleistungen 2</t>
-  </si>
-  <si>
     <t>Frauenanteil in nationalen Parlamenten</t>
+  </si>
+  <si>
+    <t>Geschlechtsspezifisches Verdienstgefälle in Industrie, Baugewerbe und Dienstleistungen 2</t>
   </si>
 </sst>
 </file>
@@ -185,7 +185,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -201,7 +201,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -500,12 +500,12 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>32</v>
       </c>
@@ -519,13 +519,13 @@
         <v>35</v>
       </c>
       <c r="E1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -542,7 +542,7 @@
         <v>41.5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -562,7 +562,7 @@
         <v>41.33</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -582,7 +582,7 @@
         <v>26.67</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -602,7 +602,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -622,7 +622,7 @@
         <v>39.659999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -642,7 +642,7 @@
         <v>31.17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -662,7 +662,7 @@
         <v>28.71</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -679,7 +679,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -696,7 +696,7 @@
         <v>21.67</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -716,7 +716,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -736,7 +736,7 @@
         <v>39.51</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -756,7 +756,7 @@
         <v>31.13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -773,7 +773,7 @@
         <v>35.71</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -793,7 +793,7 @@
         <v>19.64</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -813,7 +813,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -833,7 +833,7 @@
         <v>20.57</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -853,7 +853,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -873,7 +873,7 @@
         <v>12.06</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -893,7 +893,7 @@
         <v>13.43</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -913,7 +913,7 @@
         <v>33.33</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -933,7 +933,7 @@
         <v>39.340000000000003</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -953,7 +953,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -973,7 +973,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -993,7 +993,7 @@
         <v>21.88</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>27.78</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>22.67</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>46.99</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>33.85</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>38.1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>

</xml_diff>